<commit_message>
formatted to see useful information this time
</commit_message>
<xml_diff>
--- a/Category Data/Category Data.xlsx
+++ b/Category Data/Category Data.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\MSCS 399\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1170" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Category Sums" sheetId="1" r:id="rId1"/>
     <sheet name="Category Mean" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -146,8 +151,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +215,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -256,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,9 +301,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,6 +336,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,14 +512,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -530,7 +556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -547,16 +573,16 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.01208</v>
+        <v>-1.208E-2</v>
       </c>
       <c r="G2">
-        <v>0.34555</v>
+        <v>0.34555000000000002</v>
       </c>
       <c r="H2">
-        <v>0.01511</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>1.511E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,25 +590,25 @@
         <v>492</v>
       </c>
       <c r="C3">
-        <v>0.983</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="D3">
         <v>-1</v>
       </c>
       <c r="E3">
-        <v>-0.0015</v>
+        <v>-1.5E-3</v>
       </c>
       <c r="F3">
-        <v>-0.04483</v>
+        <v>-4.4830000000000002E-2</v>
       </c>
       <c r="G3">
         <v>0.93667</v>
       </c>
       <c r="H3">
-        <v>0.0477</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>4.7699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -590,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -602,13 +628,13 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H4">
-        <v>0.00165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1.65E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -616,13 +642,13 @@
         <v>656</v>
       </c>
       <c r="C5">
-        <v>13.05529</v>
+        <v>13.055289999999999</v>
       </c>
       <c r="D5">
         <v>-1</v>
       </c>
       <c r="E5">
-        <v>-0.00399</v>
+        <v>-3.9899999999999996E-3</v>
       </c>
       <c r="F5">
         <v>-1.52976</v>
@@ -631,10 +657,10 @@
         <v>11.52154</v>
       </c>
       <c r="H5">
-        <v>0.62144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.62143999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -648,19 +674,19 @@
         <v>-11</v>
       </c>
       <c r="E6">
-        <v>-0.031</v>
+        <v>-3.1E-2</v>
       </c>
       <c r="F6">
-        <v>-0.78349</v>
+        <v>-0.78349000000000002</v>
       </c>
       <c r="G6">
         <v>11.21322</v>
       </c>
       <c r="H6">
-        <v>0.611939999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.61193999999999904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -668,25 +694,25 @@
         <v>1579</v>
       </c>
       <c r="C7">
-        <v>1.18444</v>
+        <v>1.1844399999999999</v>
       </c>
       <c r="D7">
         <v>-1</v>
       </c>
       <c r="E7">
-        <v>-0.00135</v>
+        <v>-1.3500000000000001E-3</v>
       </c>
       <c r="F7">
-        <v>-0.06931</v>
+        <v>-6.9309999999999997E-2</v>
       </c>
       <c r="G7">
         <v>1.11405</v>
       </c>
       <c r="H7">
-        <v>0.0602</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>6.0199999999999997E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -694,25 +720,25 @@
         <v>2739</v>
       </c>
       <c r="C8">
-        <v>5.86174</v>
+        <v>5.8617400000000002</v>
       </c>
       <c r="D8">
         <v>-5</v>
       </c>
       <c r="E8">
-        <v>-0.011</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="F8">
-        <v>-0.36898</v>
+        <v>-0.36897999999999997</v>
       </c>
       <c r="G8">
-        <v>5.48176</v>
+        <v>5.4817600000000004</v>
       </c>
       <c r="H8">
-        <v>0.29971</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.29970999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -726,19 +752,19 @@
         <v>-4</v>
       </c>
       <c r="E9">
-        <v>-0.01297</v>
+        <v>-1.2970000000000001E-2</v>
       </c>
       <c r="F9">
-        <v>-0.78371</v>
+        <v>-0.78371000000000002</v>
       </c>
       <c r="G9">
-        <v>9.94015</v>
+        <v>9.9401499999999992</v>
       </c>
       <c r="H9">
-        <v>0.42897</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.42897000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -746,25 +772,25 @@
         <v>1271</v>
       </c>
       <c r="C10">
-        <v>7.64517999999999</v>
+        <v>7.6451799999999901</v>
       </c>
       <c r="D10">
         <v>-5</v>
       </c>
       <c r="E10">
-        <v>-0.05947</v>
+        <v>-5.9470000000000002E-2</v>
       </c>
       <c r="F10">
-        <v>-0.33406</v>
+        <v>-0.33406000000000002</v>
       </c>
       <c r="G10">
-        <v>7.25164999999999</v>
+        <v>7.2516499999999899</v>
       </c>
       <c r="H10">
-        <v>0.387889999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.38788999999999901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -772,25 +798,25 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D11">
         <v>-2</v>
       </c>
       <c r="E11">
-        <v>-0.036</v>
+        <v>-3.5999999999999997E-2</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H11">
-        <v>0.00099</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>9.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -807,16 +833,16 @@
         <v>-0.13</v>
       </c>
       <c r="F12">
-        <v>-0.11453</v>
+        <v>-0.11453000000000001</v>
       </c>
       <c r="G12">
-        <v>1.37206</v>
+        <v>1.3720600000000001</v>
       </c>
       <c r="H12">
-        <v>0.07547</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>7.5469999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -833,16 +859,16 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-0.04746</v>
+        <v>-4.7460000000000002E-2</v>
       </c>
       <c r="G13">
         <v>1.4417</v>
       </c>
       <c r="H13">
-        <v>0.07832</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>7.8320000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -850,7 +876,7 @@
         <v>227</v>
       </c>
       <c r="C14">
-        <v>1.46857</v>
+        <v>1.4685699999999999</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -862,13 +888,13 @@
         <v>-0.20063</v>
       </c>
       <c r="G14">
-        <v>1.26794</v>
+        <v>1.2679400000000001</v>
       </c>
       <c r="H14">
-        <v>0.06951</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>6.9510000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -885,16 +911,16 @@
         <v>-0.32</v>
       </c>
       <c r="F15">
-        <v>-0.32469</v>
+        <v>-0.32468999999999998</v>
       </c>
       <c r="G15">
-        <v>13.60231</v>
+        <v>13.602309999999999</v>
       </c>
       <c r="H15">
-        <v>0.00325</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>3.2499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -911,16 +937,16 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-0.00972</v>
+        <v>-9.7199999999999995E-3</v>
       </c>
       <c r="G16">
         <v>0.11219</v>
       </c>
       <c r="H16">
-        <v>0.00541</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>5.4099999999999999E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -928,25 +954,25 @@
         <v>8417</v>
       </c>
       <c r="C17">
-        <v>18.25576</v>
+        <v>18.255759999999999</v>
       </c>
       <c r="D17">
         <v>-21</v>
       </c>
       <c r="E17">
-        <v>-0.07241</v>
+        <v>-7.2410000000000002E-2</v>
       </c>
       <c r="F17">
-        <v>-1.07313</v>
+        <v>-1.0731299999999999</v>
       </c>
       <c r="G17">
-        <v>17.11109</v>
+        <v>17.111090000000001</v>
       </c>
       <c r="H17">
-        <v>0.68098</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>0.68098000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -954,25 +980,25 @@
         <v>2601</v>
       </c>
       <c r="C18">
-        <v>15.08294</v>
+        <v>15.082940000000001</v>
       </c>
       <c r="D18">
         <v>-21</v>
       </c>
       <c r="E18">
-        <v>-0.21166</v>
+        <v>-0.21165999999999999</v>
       </c>
       <c r="F18">
-        <v>-2.0239</v>
+        <v>-2.0238999999999998</v>
       </c>
       <c r="G18">
-        <v>12.85157</v>
+        <v>12.851570000000001</v>
       </c>
       <c r="H18">
         <v>0.67745</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -980,25 +1006,25 @@
         <v>10265</v>
       </c>
       <c r="C19">
-        <v>23.162</v>
+        <v>23.161999999999999</v>
       </c>
       <c r="D19">
         <v>-18</v>
       </c>
       <c r="E19">
-        <v>-0.041</v>
+        <v>-4.1000000000000002E-2</v>
       </c>
       <c r="F19">
-        <v>-1.48335</v>
+        <v>-1.4833499999999999</v>
       </c>
       <c r="G19">
         <v>21.6417</v>
       </c>
       <c r="H19">
-        <v>1.18758</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>1.1875800000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.78545</v>
+        <v>-0.78544999999999998</v>
       </c>
       <c r="G20">
         <v>5.0339</v>
@@ -1024,7 +1050,7 @@
         <v>0.27648</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1032,7 +1058,7 @@
         <v>6950</v>
       </c>
       <c r="C21">
-        <v>76.87371</v>
+        <v>76.873710000000003</v>
       </c>
       <c r="D21">
         <v>-93</v>
@@ -1044,13 +1070,13 @@
         <v>-6.03207</v>
       </c>
       <c r="G21">
-        <v>66.67143</v>
+        <v>66.671430000000001</v>
       </c>
       <c r="H21">
-        <v>3.28245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>3.2824499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1058,7 +1084,7 @@
         <v>12</v>
       </c>
       <c r="C22">
-        <v>0.03488</v>
+        <v>3.4880000000000001E-2</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1070,13 +1096,13 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0.03488</v>
+        <v>3.4880000000000001E-2</v>
       </c>
       <c r="H22">
-        <v>0.00191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>1.91E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1084,25 +1110,25 @@
         <v>107</v>
       </c>
       <c r="C23">
-        <v>1.21907</v>
+        <v>1.2190700000000001</v>
       </c>
       <c r="D23">
         <v>-3</v>
       </c>
       <c r="E23">
-        <v>-0.09883</v>
+        <v>-9.8830000000000001E-2</v>
       </c>
       <c r="F23">
-        <v>-0.0812</v>
+        <v>-8.1199999999999994E-2</v>
       </c>
       <c r="G23">
         <v>1.03904</v>
       </c>
       <c r="H23">
-        <v>0.02937</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>2.937E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1110,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>0.08384</v>
+        <v>8.3839999999999998E-2</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1119,16 +1145,16 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>-0.01399</v>
+        <v>-1.3990000000000001E-2</v>
       </c>
       <c r="G24">
-        <v>0.06985</v>
+        <v>6.9849999999999995E-2</v>
       </c>
       <c r="H24">
-        <v>0.00384</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>3.8400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1136,25 +1162,25 @@
         <v>914</v>
       </c>
       <c r="C25">
-        <v>5.329</v>
+        <v>5.3289999999999997</v>
       </c>
       <c r="D25">
         <v>-5</v>
       </c>
       <c r="E25">
-        <v>-0.022</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="F25">
-        <v>-0.0432</v>
+        <v>-4.3200000000000002E-2</v>
       </c>
       <c r="G25">
-        <v>5.2638</v>
+        <v>5.2637999999999998</v>
       </c>
       <c r="H25">
-        <v>0.28849</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>0.28849000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1162,16 +1188,16 @@
         <v>5907</v>
       </c>
       <c r="C26">
-        <v>36.8990999999999</v>
+        <v>36.899099999999898</v>
       </c>
       <c r="D26">
         <v>-62</v>
       </c>
       <c r="E26">
-        <v>-1.7213</v>
+        <v>-1.7213000000000001</v>
       </c>
       <c r="F26">
-        <v>-5.62664</v>
+        <v>-5.6266400000000001</v>
       </c>
       <c r="G26">
         <v>29.55752</v>
@@ -1180,7 +1206,7 @@
         <v>1.57233</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1188,25 +1214,25 @@
         <v>1150</v>
       </c>
       <c r="C27">
-        <v>8.83377</v>
+        <v>8.8337699999999995</v>
       </c>
       <c r="D27">
         <v>-11</v>
       </c>
       <c r="E27">
-        <v>-0.16364</v>
+        <v>-0.16364000000000001</v>
       </c>
       <c r="F27">
         <v>-1.21044</v>
       </c>
       <c r="G27">
-        <v>7.45969</v>
+        <v>7.4596900000000002</v>
       </c>
       <c r="H27">
-        <v>0.36969</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0.36969000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1214,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>0.135</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D28">
         <v>-1</v>
@@ -1223,7 +1249,7 @@
         <v>-0.1</v>
       </c>
       <c r="F28">
-        <v>-0.035</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1232,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1240,7 +1266,7 @@
         <v>74</v>
       </c>
       <c r="C29">
-        <v>1.58122</v>
+        <v>1.5812200000000001</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1249,16 +1275,16 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>-0.06811</v>
+        <v>-6.8110000000000004E-2</v>
       </c>
       <c r="G29">
         <v>1.51311</v>
       </c>
       <c r="H29">
-        <v>0.08324</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>8.3239999999999995E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1266,25 +1292,25 @@
         <v>1138</v>
       </c>
       <c r="C30">
-        <v>5.94413</v>
+        <v>5.9441300000000004</v>
       </c>
       <c r="D30">
         <v>-18</v>
       </c>
       <c r="E30">
-        <v>-0.19933</v>
+        <v>-0.19933000000000001</v>
       </c>
       <c r="F30">
         <v>-0.31633</v>
       </c>
       <c r="G30">
-        <v>5.43347</v>
+        <v>5.4334699999999998</v>
       </c>
       <c r="H30">
-        <v>0.18382</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0.18382000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1310,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1318,16 +1344,16 @@
         <v>190</v>
       </c>
       <c r="C32">
-        <v>0.199</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="D32">
         <v>-3</v>
       </c>
       <c r="E32">
-        <v>-0.003</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="F32">
-        <v>-0.01047</v>
+        <v>-1.047E-2</v>
       </c>
       <c r="G32">
         <v>0.18553</v>
@@ -1336,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1344,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <v>0.09998</v>
+        <v>9.9979999999999999E-2</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1353,16 +1379,16 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>-0.0363</v>
+        <v>-3.6299999999999999E-2</v>
       </c>
       <c r="G33">
-        <v>0.06368</v>
+        <v>6.368E-2</v>
       </c>
       <c r="H33">
-        <v>0.0035</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1370,25 +1396,25 @@
         <v>101</v>
       </c>
       <c r="C34">
-        <v>2.1087</v>
+        <v>2.1086999999999998</v>
       </c>
       <c r="D34">
         <v>-2</v>
       </c>
       <c r="E34">
-        <v>-0.06925</v>
+        <v>-6.9250000000000006E-2</v>
       </c>
       <c r="F34">
-        <v>-0.36084</v>
+        <v>-0.36083999999999999</v>
       </c>
       <c r="G34">
         <v>1.69049</v>
       </c>
       <c r="H34">
-        <v>0.07886</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>7.886E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1396,38 +1422,246 @@
         <v>2032</v>
       </c>
       <c r="C35">
-        <v>8.76522</v>
+        <v>8.7652199999999993</v>
       </c>
       <c r="D35">
         <v>-1</v>
       </c>
       <c r="E35">
-        <v>-0.00399</v>
+        <v>-3.9899999999999996E-3</v>
       </c>
       <c r="F35">
-        <v>-0.64192</v>
+        <v>-0.64192000000000005</v>
       </c>
       <c r="G35">
-        <v>8.11931</v>
+        <v>8.1193100000000005</v>
       </c>
       <c r="H35">
-        <v>0.40928</v>
+        <v>0.40927999999999998</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1E221E88-74E5-4EE2-9E44-E7E342E9D173}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B65E8553-8F14-4A24-BEAD-742C2E49D1BB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F419C689-BA1F-4590-B38A-753EB489FCC6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DF6808AF-5857-4739-9CF3-6803E0ECE537}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D8EF9222-8DC2-42D3-8CFD-99D4C85959D1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C645BE00-4300-4719-9073-304111BD748A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{421A1998-EDAD-4E8D-A0B2-3DFC3D06CBDB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1E221E88-74E5-4EE2-9E44-E7E342E9D173}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B65E8553-8F14-4A24-BEAD-742C2E49D1BB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F419C689-BA1F-4590-B38A-753EB489FCC6}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DF6808AF-5857-4739-9CF3-6803E0ECE537}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D8EF9222-8DC2-42D3-8CFD-99D4C85959D1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C645BE00-4300-4719-9073-304111BD748A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{421A1998-EDAD-4E8D-A0B2-3DFC3D06CBDB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1453,7 +1687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1470,42 +1704,42 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.01208</v>
+        <v>-1.208E-2</v>
       </c>
       <c r="G2">
-        <v>0.34555</v>
+        <v>0.34555000000000002</v>
       </c>
       <c r="H2">
-        <v>0.01511</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>1.511E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>12.6153846153846</v>
+        <v>12.615384615384601</v>
       </c>
       <c r="C3">
-        <v>0.0252051282051282</v>
+        <v>2.5205128205128199E-2</v>
       </c>
       <c r="D3">
-        <v>-0.0256410256410256</v>
+        <v>-2.5641025641025599E-2</v>
       </c>
       <c r="E3">
-        <v>-3.84615384615385e-05</v>
+        <v>-3.8461538461538497E-5</v>
       </c>
       <c r="F3">
-        <v>-0.00114948717948718</v>
+        <v>-1.1494871794871799E-3</v>
       </c>
       <c r="G3">
-        <v>0.0240171794871795</v>
+        <v>2.4017179487179501E-2</v>
       </c>
       <c r="H3">
-        <v>0.00122307692307692</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>1.22307692307692E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1513,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1525,39 +1759,39 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H4">
-        <v>0.00165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1.65E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5">
-        <v>2.73333333333333</v>
+        <v>2.7333333333333298</v>
       </c>
       <c r="C5">
-        <v>0.0543970416666666</v>
+        <v>5.4397041666666597E-2</v>
       </c>
       <c r="D5">
-        <v>-0.00416666666666667</v>
+        <v>-4.1666666666666701E-3</v>
       </c>
       <c r="E5">
-        <v>-1.6625e-05</v>
+        <v>-1.6625000000000001E-5</v>
       </c>
       <c r="F5">
-        <v>-0.006374</v>
+        <v>-6.3740000000000003E-3</v>
       </c>
       <c r="G5">
-        <v>0.0480064166666666</v>
+        <v>4.80064166666666E-2</v>
       </c>
       <c r="H5">
-        <v>0.00258933333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>2.5893333333333302E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1565,77 +1799,77 @@
         <v>14.9772727272727</v>
       </c>
       <c r="C6">
-        <v>0.0341640909090908</v>
+        <v>3.4164090909090797E-2</v>
       </c>
       <c r="D6">
-        <v>-0.03125</v>
+        <v>-3.125E-2</v>
       </c>
       <c r="E6">
-        <v>-8.80681818181818e-05</v>
+        <v>-8.8068181818181805E-5</v>
       </c>
       <c r="F6">
-        <v>-0.00222582386363636</v>
+        <v>-2.2258238636363599E-3</v>
       </c>
       <c r="G6">
-        <v>0.0318557386363636</v>
+        <v>3.1855738636363602E-2</v>
       </c>
       <c r="H6">
-        <v>0.00173846590909091</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>1.73846590909091E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <v>26.3166666666667</v>
+        <v>26.316666666666698</v>
       </c>
       <c r="C7">
-        <v>0.0197406666666667</v>
+        <v>1.9740666666666701E-2</v>
       </c>
       <c r="D7">
-        <v>-0.0166666666666667</v>
+        <v>-1.6666666666666701E-2</v>
       </c>
       <c r="E7">
-        <v>-2.25e-05</v>
+        <v>-2.2500000000000001E-5</v>
       </c>
       <c r="F7">
-        <v>-0.00115516666666667</v>
+        <v>-1.15516666666667E-3</v>
       </c>
       <c r="G7">
-        <v>0.0185675</v>
+        <v>1.8567500000000001E-2</v>
       </c>
       <c r="H7">
-        <v>0.00100333333333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>1.00333333333333E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8">
-        <v>34.6708860759494</v>
+        <v>34.670886075949397</v>
       </c>
       <c r="C8">
-        <v>0.0741992405063291</v>
+        <v>7.4199240506329103E-2</v>
       </c>
       <c r="D8">
-        <v>-0.0632911392405063</v>
+        <v>-6.3291139240506306E-2</v>
       </c>
       <c r="E8">
-        <v>-0.000139240506329114</v>
+        <v>-1.39240506329114E-4</v>
       </c>
       <c r="F8">
-        <v>-0.00467063291139241</v>
+        <v>-4.6706329113924104E-3</v>
       </c>
       <c r="G8">
-        <v>0.0693893670886076</v>
+        <v>6.9389367088607601E-2</v>
       </c>
       <c r="H8">
-        <v>0.00379379746835443</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>3.7937974683544301E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1646,48 +1880,48 @@
         <v>0.155544637681159</v>
       </c>
       <c r="D9">
-        <v>-0.0579710144927536</v>
+        <v>-5.7971014492753603E-2</v>
       </c>
       <c r="E9">
-        <v>-0.000187971014492754</v>
+        <v>-1.87971014492754E-4</v>
       </c>
       <c r="F9">
-        <v>-0.011358115942029</v>
+        <v>-1.1358115942029E-2</v>
       </c>
       <c r="G9">
-        <v>0.144060144927536</v>
+        <v>0.14406014492753599</v>
       </c>
       <c r="H9">
-        <v>0.00621695652173913</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>6.2169565217391302E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10">
-        <v>4.29391891891892</v>
+        <v>4.2939189189189202</v>
       </c>
       <c r="C10">
-        <v>0.0258283108108108</v>
+        <v>2.5828310810810801E-2</v>
       </c>
       <c r="D10">
-        <v>-0.0168918918918919</v>
+        <v>-1.68918918918919E-2</v>
       </c>
       <c r="E10">
-        <v>-0.000200912162162162</v>
+        <v>-2.0091216216216201E-4</v>
       </c>
       <c r="F10">
-        <v>-0.00112858108108108</v>
+        <v>-1.12858108108108E-3</v>
       </c>
       <c r="G10">
-        <v>0.0244988175675675</v>
+        <v>2.4498817567567499E-2</v>
       </c>
       <c r="H10">
-        <v>0.00131043918918918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>1.31043918918918E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1695,51 +1929,51 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="D11">
         <v>-2</v>
       </c>
       <c r="E11">
-        <v>-0.036</v>
+        <v>-3.5999999999999997E-2</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H11">
-        <v>0.00099</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>9.8999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12">
-        <v>4.68421052631579</v>
+        <v>4.6842105263157903</v>
       </c>
       <c r="C12">
-        <v>0.0850836842105263</v>
+        <v>8.5083684210526297E-2</v>
       </c>
       <c r="D12">
-        <v>-0.0526315789473684</v>
+        <v>-5.2631578947368397E-2</v>
       </c>
       <c r="E12">
-        <v>-0.0068421052631579</v>
+        <v>-6.8421052631579002E-3</v>
       </c>
       <c r="F12">
-        <v>-0.0060278947368421</v>
+        <v>-6.0278947368421001E-3</v>
       </c>
       <c r="G12">
-        <v>0.0722136842105263</v>
+        <v>7.2213684210526305E-2</v>
       </c>
       <c r="H12">
-        <v>0.00397210526315789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>3.9721052631578897E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1747,7 +1981,7 @@
         <v>25.75</v>
       </c>
       <c r="C13">
-        <v>0.04653625</v>
+        <v>4.6536250000000001E-2</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1756,24 +1990,24 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-0.001483125</v>
+        <v>-1.4831250000000001E-3</v>
       </c>
       <c r="G13">
-        <v>0.045053125</v>
+        <v>4.5053124999999999E-2</v>
       </c>
       <c r="H13">
-        <v>0.0024475</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>2.4475E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14">
-        <v>20.6363636363636</v>
+        <v>20.636363636363601</v>
       </c>
       <c r="C14">
-        <v>0.133506363636364</v>
+        <v>0.13350636363636401</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1782,42 +2016,42 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>-0.0182390909090909</v>
+        <v>-1.8239090909090899E-2</v>
       </c>
       <c r="G14">
         <v>0.115267272727273</v>
       </c>
       <c r="H14">
-        <v>0.00631909090909091</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>6.3190909090909096E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15">
-        <v>49.4242424242424</v>
+        <v>49.424242424242401</v>
       </c>
       <c r="C15">
-        <v>0.431727272727273</v>
+        <v>0.43172727272727301</v>
       </c>
       <c r="D15">
-        <v>-0.575757575757576</v>
+        <v>-0.57575757575757602</v>
       </c>
       <c r="E15">
-        <v>-0.0096969696969697</v>
+        <v>-9.6969696969697004E-3</v>
       </c>
       <c r="F15">
-        <v>-0.00983909090909091</v>
+        <v>-9.8390909090909102E-3</v>
       </c>
       <c r="G15">
-        <v>0.412191212121212</v>
+        <v>0.41219121212121201</v>
       </c>
       <c r="H15">
-        <v>9.84848484848485e-05</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>9.8484848484848504E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1825,7 +2059,7 @@
         <v>1.5</v>
       </c>
       <c r="C16">
-        <v>0.0203183333333333</v>
+        <v>2.0318333333333299E-2</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1834,42 +2068,42 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-0.00162</v>
+        <v>-1.6199999999999999E-3</v>
       </c>
       <c r="G16">
-        <v>0.0186983333333333</v>
+        <v>1.8698333333333299E-2</v>
       </c>
       <c r="H16">
-        <v>0.000901666666666667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>9.0166666666666704E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17">
-        <v>40.6618357487923</v>
+        <v>40.661835748792299</v>
       </c>
       <c r="C17">
-        <v>0.088192077294686</v>
+        <v>8.8192077294686005E-2</v>
       </c>
       <c r="D17">
         <v>-0.101449275362319</v>
       </c>
       <c r="E17">
-        <v>-0.000349806763285024</v>
+        <v>-3.4980676328502398E-4</v>
       </c>
       <c r="F17">
-        <v>-0.00518420289855072</v>
+        <v>-5.1842028985507197E-3</v>
       </c>
       <c r="G17">
-        <v>0.082662270531401</v>
+        <v>8.2662270531401003E-2</v>
       </c>
       <c r="H17">
-        <v>0.00328975845410628</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>3.2897584541062802E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1877,51 +2111,51 @@
         <v>76.5</v>
       </c>
       <c r="C18">
-        <v>0.443615882352941</v>
+        <v>0.44361588235294103</v>
       </c>
       <c r="D18">
-        <v>-0.617647058823529</v>
+        <v>-0.61764705882352899</v>
       </c>
       <c r="E18">
-        <v>-0.00622529411764706</v>
+        <v>-6.2252941176470598E-3</v>
       </c>
       <c r="F18">
-        <v>-0.0595264705882353</v>
+        <v>-5.9526470588235299E-2</v>
       </c>
       <c r="G18">
-        <v>0.377987352941176</v>
+        <v>0.37798735294117602</v>
       </c>
       <c r="H18">
-        <v>0.019925</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>1.9924999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B19">
-        <v>46.2387387387387</v>
+        <v>46.238738738738697</v>
       </c>
       <c r="C19">
         <v>0.104333333333333</v>
       </c>
       <c r="D19">
-        <v>-0.0810810810810811</v>
+        <v>-8.1081081081081099E-2</v>
       </c>
       <c r="E19">
-        <v>-0.000184684684684685</v>
+        <v>-1.8468468468468499E-4</v>
       </c>
       <c r="F19">
-        <v>-0.00668175675675675</v>
+        <v>-6.6817567567567498E-3</v>
       </c>
       <c r="G19">
-        <v>0.0974851351351351</v>
+        <v>9.7485135135135098E-2</v>
       </c>
       <c r="H19">
-        <v>0.00534945945945946</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>5.34945945945946E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1938,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.392725</v>
+        <v>-0.39272499999999999</v>
       </c>
       <c r="G20">
         <v>2.51695</v>
@@ -1947,33 +2181,33 @@
         <v>0.13824</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B21">
-        <v>76.3736263736264</v>
+        <v>76.373626373626394</v>
       </c>
       <c r="C21">
-        <v>0.844766043956044</v>
+        <v>0.84476604395604404</v>
       </c>
       <c r="D21">
-        <v>-1.02197802197802</v>
+        <v>-1.0219780219780199</v>
       </c>
       <c r="E21">
-        <v>-0.0459092307692308</v>
+        <v>-4.5909230769230799E-2</v>
       </c>
       <c r="F21">
-        <v>-0.0662864835164835</v>
+        <v>-6.6286483516483502E-2</v>
       </c>
       <c r="G21">
-        <v>0.732653076923077</v>
+        <v>0.73265307692307702</v>
       </c>
       <c r="H21">
-        <v>0.0360708791208791</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>3.6070879120879099E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1981,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0.00290666666666667</v>
+        <v>2.9066666666666698E-3</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1993,13 +2227,13 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0.00290666666666667</v>
+        <v>2.9066666666666698E-3</v>
       </c>
       <c r="H22">
-        <v>0.000159166666666667</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>1.5916666666666699E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2013,19 +2247,19 @@
         <v>-0.3</v>
       </c>
       <c r="E23">
-        <v>-0.009883</v>
+        <v>-9.8829999999999994E-3</v>
       </c>
       <c r="F23">
-        <v>-0.00812</v>
+        <v>-8.1200000000000005E-3</v>
       </c>
       <c r="G23">
         <v>0.103904</v>
       </c>
       <c r="H23">
-        <v>0.002937</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>2.9369999999999999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2033,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0.02096</v>
+        <v>2.0959999999999999E-2</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2042,16 +2276,16 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>-0.0034975</v>
+        <v>-3.4975000000000002E-3</v>
       </c>
       <c r="G24">
-        <v>0.0174625</v>
+        <v>1.7462499999999999E-2</v>
       </c>
       <c r="H24">
-        <v>0.00096</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>9.6000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -2059,25 +2293,25 @@
         <v>228.5</v>
       </c>
       <c r="C25">
-        <v>1.33225</v>
+        <v>1.3322499999999999</v>
       </c>
       <c r="D25">
         <v>-1.25</v>
       </c>
       <c r="E25">
-        <v>-0.0055</v>
+        <v>-5.4999999999999997E-3</v>
       </c>
       <c r="F25">
-        <v>-0.0108</v>
+        <v>-1.0800000000000001E-2</v>
       </c>
       <c r="G25">
         <v>1.31595</v>
       </c>
       <c r="H25">
-        <v>0.0721225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>7.2122500000000006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2085,68 +2319,68 @@
         <v>13.2443946188341</v>
       </c>
       <c r="C26">
-        <v>0.0827334080717487</v>
+        <v>8.2733408071748699E-2</v>
       </c>
       <c r="D26">
         <v>-0.139013452914798</v>
       </c>
       <c r="E26">
-        <v>-0.00385941704035874</v>
+        <v>-3.8594170403587402E-3</v>
       </c>
       <c r="F26">
-        <v>-0.0126157847533632</v>
+        <v>-1.26157847533632E-2</v>
       </c>
       <c r="G26">
-        <v>0.066272466367713</v>
+        <v>6.6272466367713001E-2</v>
       </c>
       <c r="H26">
-        <v>0.00352540358744395</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>3.5254035874439501E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B27">
-        <v>20.5357142857143</v>
+        <v>20.535714285714299</v>
       </c>
       <c r="C27">
-        <v>0.157745892857143</v>
+        <v>0.15774589285714299</v>
       </c>
       <c r="D27">
-        <v>-0.196428571428571</v>
+        <v>-0.19642857142857101</v>
       </c>
       <c r="E27">
-        <v>-0.00292214285714286</v>
+        <v>-2.9221428571428601E-3</v>
       </c>
       <c r="F27">
-        <v>-0.021615</v>
+        <v>-2.1614999999999999E-2</v>
       </c>
       <c r="G27">
-        <v>0.13320875</v>
+        <v>0.13320874999999999</v>
       </c>
       <c r="H27">
-        <v>0.00660160714285714</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>6.60160714285714E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28">
-        <v>1.33333333333333</v>
+        <v>1.3333333333333299</v>
       </c>
       <c r="C28">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D28">
-        <v>-0.333333333333333</v>
+        <v>-0.33333333333333298</v>
       </c>
       <c r="E28">
-        <v>-0.0333333333333333</v>
+        <v>-3.3333333333333298E-2</v>
       </c>
       <c r="F28">
-        <v>-0.0116666666666667</v>
+        <v>-1.16666666666667E-2</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -2155,15 +2389,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B29">
-        <v>2.05555555555556</v>
+        <v>2.0555555555555598</v>
       </c>
       <c r="C29">
-        <v>0.0439227777777778</v>
+        <v>4.3922777777777797E-2</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2172,16 +2406,16 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>-0.00189194444444444</v>
+        <v>-1.89194444444444E-3</v>
       </c>
       <c r="G29">
-        <v>0.0420308333333333</v>
+        <v>4.2030833333333302E-2</v>
       </c>
       <c r="H29">
-        <v>0.00231222222222222</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>2.3122222222222199E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2189,25 +2423,25 @@
         <v>13.8780487804878</v>
       </c>
       <c r="C30">
-        <v>0.0724893902439024</v>
+        <v>7.2489390243902399E-2</v>
       </c>
       <c r="D30">
         <v>-0.219512195121951</v>
       </c>
       <c r="E30">
-        <v>-0.00243085365853659</v>
+        <v>-2.43085365853659E-3</v>
       </c>
       <c r="F30">
-        <v>-0.00385768292682927</v>
+        <v>-3.8576829268292699E-3</v>
       </c>
       <c r="G30">
-        <v>0.0662618292682926</v>
+        <v>6.6261829268292605E-2</v>
       </c>
       <c r="H30">
-        <v>0.00224170731707317</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>2.2417073170731701E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2233,7 +2467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2241,25 +2475,25 @@
         <v>95</v>
       </c>
       <c r="C32">
-        <v>0.0995</v>
+        <v>9.9500000000000005E-2</v>
       </c>
       <c r="D32">
         <v>-1.5</v>
       </c>
       <c r="E32">
-        <v>-0.0015</v>
+        <v>-1.5E-3</v>
       </c>
       <c r="F32">
-        <v>-0.005235</v>
+        <v>-5.2350000000000001E-3</v>
       </c>
       <c r="G32">
-        <v>0.092765</v>
+        <v>9.2765E-2</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2267,7 +2501,7 @@
         <v>2</v>
       </c>
       <c r="C33">
-        <v>0.09998</v>
+        <v>9.9979999999999999E-2</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2276,16 +2510,16 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>-0.0363</v>
+        <v>-3.6299999999999999E-2</v>
       </c>
       <c r="G33">
-        <v>0.06368</v>
+        <v>6.368E-2</v>
       </c>
       <c r="H33">
-        <v>0.0035</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>3.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -2293,51 +2527,271 @@
         <v>1.62903225806452</v>
       </c>
       <c r="C34">
-        <v>0.0340112903225807</v>
+        <v>3.4011290322580698E-2</v>
       </c>
       <c r="D34">
-        <v>-0.032258064516129</v>
+        <v>-3.2258064516128997E-2</v>
       </c>
       <c r="E34">
-        <v>-0.00111693548387097</v>
+        <v>-1.1169354838709701E-3</v>
       </c>
       <c r="F34">
-        <v>-0.00582</v>
+        <v>-5.8199999999999997E-3</v>
       </c>
       <c r="G34">
-        <v>0.0272659677419355</v>
+        <v>2.7265967741935501E-2</v>
       </c>
       <c r="H34">
-        <v>0.00127193548387097</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>1.2719354838709701E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B35">
-        <v>72.5714285714286</v>
+        <v>72.571428571428598</v>
       </c>
       <c r="C35">
-        <v>0.313043571428571</v>
+        <v>0.31304357142857098</v>
       </c>
       <c r="D35">
-        <v>-0.0357142857142857</v>
+        <v>-3.5714285714285698E-2</v>
       </c>
       <c r="E35">
-        <v>-0.0001425</v>
+        <v>-1.4249999999999999E-4</v>
       </c>
       <c r="F35">
-        <v>-0.0229257142857143</v>
+        <v>-2.2925714285714299E-2</v>
       </c>
       <c r="G35">
-        <v>0.289975357142857</v>
+        <v>0.28997535714285699</v>
       </c>
       <c r="H35">
-        <v>0.0146171428571429</v>
+        <v>1.46171428571429E-2</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:G35">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EB14C052-B622-464B-8B40-5F0F7F79E1A2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A12EFE6B-B2C3-48CF-8BFD-170E9686368A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C270B6E5-FAB4-4F62-9D86-FFCA2B2B04D8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E9E97897-B700-47E5-860F-F3FCE592CFB9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{36D5F5BD-42D3-430D-A434-44ADCB6F51E2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{350DDAB0-0AD8-4CE9-9BE4-CDDF938C1989}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FA85B461-3F2D-4415-A7E4-97F5C9FB20A8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{91BCFD64-C5CE-462A-AAC9-B56ACA4B4EA4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EB14C052-B622-464B-8B40-5F0F7F79E1A2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G2:G35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A12EFE6B-B2C3-48CF-8BFD-170E9686368A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C270B6E5-FAB4-4F62-9D86-FFCA2B2B04D8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E9E97897-B700-47E5-860F-F3FCE592CFB9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{36D5F5BD-42D3-430D-A434-44ADCB6F51E2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{350DDAB0-0AD8-4CE9-9BE4-CDDF938C1989}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FA85B461-3F2D-4415-A7E4-97F5C9FB20A8}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{91BCFD64-C5CE-462A-AAC9-B56ACA4B4EA4}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
good data this time
</commit_message>
<xml_diff>
--- a/Category Data/Category Data.xlsx
+++ b/Category Data/Category Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\MSCS 399\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Student Data\Documents\GitHub\TheDistrictCompany\Category Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2100" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Category Sums" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Items Sold</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Yu-Gi-Oh</t>
+  </si>
+  <si>
+    <t>MTGSealed(Booster,Fat packs)</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -1645,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,10 +1695,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>0.114285714285714</v>
       </c>
       <c r="C2">
-        <v>0.35763</v>
+        <v>1.4597142857142901E-3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1704,13 +1707,13 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-1.208E-2</v>
+        <v>-4.9306122448979598E-5</v>
       </c>
       <c r="G2">
-        <v>0.34555000000000002</v>
+        <v>1.4104081632653101E-3</v>
       </c>
       <c r="H2">
-        <v>1.511E-2</v>
+        <v>6.1673469387755095E-5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1718,25 +1721,25 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>12.615384615384601</v>
+        <v>2.0081632653061199</v>
       </c>
       <c r="C3">
-        <v>2.5205128205128199E-2</v>
+        <v>4.0122448979591904E-3</v>
       </c>
       <c r="D3">
-        <v>-2.5641025641025599E-2</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E3">
-        <v>-3.8461538461538497E-5</v>
+        <v>-6.1224489795918396E-6</v>
       </c>
       <c r="F3">
-        <v>-1.1494871794871799E-3</v>
+        <v>-1.82979591836735E-4</v>
       </c>
       <c r="G3">
-        <v>2.4017179487179501E-2</v>
+        <v>3.82314285714286E-3</v>
       </c>
       <c r="H3">
-        <v>1.22307692307692E-3</v>
+        <v>1.9469387755102001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,10 +1747,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1.2244897959183701E-2</v>
       </c>
       <c r="C4">
-        <v>0.14000000000000001</v>
+        <v>5.7142857142857104E-4</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1759,10 +1762,10 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.14000000000000001</v>
+        <v>5.7142857142857104E-4</v>
       </c>
       <c r="H4">
-        <v>1.65E-3</v>
+        <v>6.7346938775510201E-6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1770,25 +1773,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>2.7333333333333298</v>
+        <v>2.6775510204081598</v>
       </c>
       <c r="C5">
-        <v>5.4397041666666597E-2</v>
+        <v>5.32868979591836E-2</v>
       </c>
       <c r="D5">
-        <v>-4.1666666666666701E-3</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E5">
-        <v>-1.6625000000000001E-5</v>
+        <v>-1.62857142857143E-5</v>
       </c>
       <c r="F5">
-        <v>-6.3740000000000003E-3</v>
+        <v>-6.2439183673469404E-3</v>
       </c>
       <c r="G5">
-        <v>4.80064166666666E-2</v>
+        <v>4.7026693877550999E-2</v>
       </c>
       <c r="H5">
-        <v>2.5893333333333302E-3</v>
+        <v>2.5364897959183701E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1796,25 +1799,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>14.9772727272727</v>
+        <v>21.518367346938799</v>
       </c>
       <c r="C6">
-        <v>3.4164090909090797E-2</v>
+        <v>4.9084734693877502E-2</v>
       </c>
       <c r="D6">
-        <v>-3.125E-2</v>
+        <v>-4.4897959183673501E-2</v>
       </c>
       <c r="E6">
-        <v>-8.8068181818181805E-5</v>
+        <v>-1.2653061224489801E-4</v>
       </c>
       <c r="F6">
-        <v>-2.2258238636363599E-3</v>
+        <v>-3.1979183673469399E-3</v>
       </c>
       <c r="G6">
-        <v>3.1855738636363602E-2</v>
+        <v>4.57682448979592E-2</v>
       </c>
       <c r="H6">
-        <v>1.73846590909091E-3</v>
+        <v>2.4977142857142802E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1822,25 +1825,25 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>26.316666666666698</v>
+        <v>6.4448979591836704</v>
       </c>
       <c r="C7">
-        <v>1.9740666666666701E-2</v>
+        <v>4.8344489795918303E-3</v>
       </c>
       <c r="D7">
-        <v>-1.6666666666666701E-2</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E7">
-        <v>-2.2500000000000001E-5</v>
+        <v>-5.5102040816326498E-6</v>
       </c>
       <c r="F7">
-        <v>-1.15516666666667E-3</v>
+        <v>-2.82897959183674E-4</v>
       </c>
       <c r="G7">
-        <v>1.8567500000000001E-2</v>
+        <v>4.5471428571428503E-3</v>
       </c>
       <c r="H7">
-        <v>1.00333333333333E-3</v>
+        <v>2.4571428571428601E-4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1848,25 +1851,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>34.670886075949397</v>
+        <v>11.1795918367347</v>
       </c>
       <c r="C8">
-        <v>7.4199240506329103E-2</v>
+        <v>2.39254693877551E-2</v>
       </c>
       <c r="D8">
-        <v>-6.3291139240506306E-2</v>
+        <v>-2.04081632653061E-2</v>
       </c>
       <c r="E8">
-        <v>-1.39240506329114E-4</v>
+        <v>-4.4897959183673501E-5</v>
       </c>
       <c r="F8">
-        <v>-4.6706329113924104E-3</v>
+        <v>-1.50604081632653E-3</v>
       </c>
       <c r="G8">
-        <v>6.9389367088607601E-2</v>
+        <v>2.2374530612244901E-2</v>
       </c>
       <c r="H8">
-        <v>3.7937974683544301E-3</v>
+        <v>1.22330612244898E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1874,25 +1877,25 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>31.9710144927536</v>
+        <v>9.0040816326530599</v>
       </c>
       <c r="C9">
-        <v>0.155544637681159</v>
+        <v>4.3806448979591801E-2</v>
       </c>
       <c r="D9">
-        <v>-5.7971014492753603E-2</v>
+        <v>-1.6326530612244899E-2</v>
       </c>
       <c r="E9">
-        <v>-1.87971014492754E-4</v>
+        <v>-5.2938775510204103E-5</v>
       </c>
       <c r="F9">
-        <v>-1.1358115942029E-2</v>
+        <v>-3.19881632653061E-3</v>
       </c>
       <c r="G9">
-        <v>0.14406014492753599</v>
+        <v>4.0572040816326503E-2</v>
       </c>
       <c r="H9">
-        <v>6.2169565217391302E-3</v>
+        <v>1.7508979591836699E-3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1900,25 +1903,25 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>4.2939189189189202</v>
+        <v>5.1877551020408204</v>
       </c>
       <c r="C10">
-        <v>2.5828310810810801E-2</v>
+        <v>3.1204816326530601E-2</v>
       </c>
       <c r="D10">
-        <v>-1.68918918918919E-2</v>
+        <v>-2.04081632653061E-2</v>
       </c>
       <c r="E10">
-        <v>-2.0091216216216201E-4</v>
+        <v>-2.42734693877551E-4</v>
       </c>
       <c r="F10">
-        <v>-1.12858108108108E-3</v>
+        <v>-1.3635102040816299E-3</v>
       </c>
       <c r="G10">
-        <v>2.4498817567567499E-2</v>
+        <v>2.9598571428571401E-2</v>
       </c>
       <c r="H10">
-        <v>1.31043918918918E-3</v>
+        <v>1.58322448979591E-3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1926,25 +1929,25 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>1.2244897959183701E-2</v>
       </c>
       <c r="C11">
-        <v>5.3999999999999999E-2</v>
+        <v>2.2040816326530601E-4</v>
       </c>
       <c r="D11">
-        <v>-2</v>
+        <v>-8.1632653061224497E-3</v>
       </c>
       <c r="E11">
-        <v>-3.5999999999999997E-2</v>
+        <v>-1.4693877551020401E-4</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1.7999999999999999E-2</v>
+        <v>7.3469387755102005E-5</v>
       </c>
       <c r="H11">
-        <v>9.8999999999999999E-4</v>
+        <v>4.0408163265306099E-6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1952,25 +1955,25 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>4.6842105263157903</v>
+        <v>0.36326530612244901</v>
       </c>
       <c r="C12">
-        <v>8.5083684210526297E-2</v>
+        <v>6.5983265306122502E-3</v>
       </c>
       <c r="D12">
-        <v>-5.2631578947368397E-2</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E12">
-        <v>-6.8421052631579002E-3</v>
+        <v>-5.3061224489795898E-4</v>
       </c>
       <c r="F12">
-        <v>-6.0278947368421001E-3</v>
+        <v>-4.6746938775510199E-4</v>
       </c>
       <c r="G12">
-        <v>7.2213684210526305E-2</v>
+        <v>5.6002448979591904E-3</v>
       </c>
       <c r="H12">
-        <v>3.9721052631578897E-3</v>
+        <v>3.0804081632653099E-4</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1978,10 +1981,10 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>25.75</v>
+        <v>3.3632653061224498</v>
       </c>
       <c r="C13">
-        <v>4.6536250000000001E-2</v>
+        <v>6.0782040816326497E-3</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1990,13 +1993,13 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>-1.4831250000000001E-3</v>
+        <v>-1.9371428571428599E-4</v>
       </c>
       <c r="G13">
-        <v>4.5053124999999999E-2</v>
+        <v>5.88448979591837E-3</v>
       </c>
       <c r="H13">
-        <v>2.4475E-3</v>
+        <v>3.1967346938775498E-4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2004,10 +2007,10 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>20.636363636363601</v>
+        <v>0.92653061224489797</v>
       </c>
       <c r="C14">
-        <v>0.13350636363636401</v>
+        <v>5.9941632653061202E-3</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2016,13 +2019,13 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>-1.8239090909090899E-2</v>
+        <v>-8.1889795918367299E-4</v>
       </c>
       <c r="G14">
-        <v>0.115267272727273</v>
+        <v>5.1752653061224504E-3</v>
       </c>
       <c r="H14">
-        <v>6.3190909090909096E-3</v>
+        <v>2.8371428571428601E-4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2030,25 +2033,25 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>49.424242424242401</v>
+        <v>6.6571428571428601</v>
       </c>
       <c r="C15">
-        <v>0.43172727272727301</v>
+        <v>5.8151020408163299E-2</v>
       </c>
       <c r="D15">
-        <v>-0.57575757575757602</v>
+        <v>-7.7551020408163293E-2</v>
       </c>
       <c r="E15">
-        <v>-9.6969696969697004E-3</v>
+        <v>-1.3061224489795901E-3</v>
       </c>
       <c r="F15">
-        <v>-9.8390909090909102E-3</v>
+        <v>-1.32526530612245E-3</v>
       </c>
       <c r="G15">
-        <v>0.41219121212121201</v>
+        <v>5.5519632653061202E-2</v>
       </c>
       <c r="H15">
-        <v>9.8484848484848504E-5</v>
+        <v>1.3265306122449E-5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2056,10 +2059,10 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>3.6734693877551003E-2</v>
       </c>
       <c r="C16">
-        <v>2.0318333333333299E-2</v>
+        <v>4.9759183673469404E-4</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2068,13 +2071,13 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>-1.6199999999999999E-3</v>
+        <v>-3.9673469387755102E-5</v>
       </c>
       <c r="G16">
-        <v>1.8698333333333299E-2</v>
+        <v>4.5791836734693898E-4</v>
       </c>
       <c r="H16">
-        <v>9.0166666666666704E-4</v>
+        <v>2.2081632653061199E-5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2082,25 +2085,25 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>40.661835748792299</v>
+        <v>34.355102040816298</v>
       </c>
       <c r="C17">
-        <v>8.8192077294686005E-2</v>
+        <v>7.4513306122448997E-2</v>
       </c>
       <c r="D17">
-        <v>-0.101449275362319</v>
+        <v>-8.5714285714285701E-2</v>
       </c>
       <c r="E17">
-        <v>-3.4980676328502398E-4</v>
+        <v>-2.9555102040816302E-4</v>
       </c>
       <c r="F17">
-        <v>-5.1842028985507197E-3</v>
+        <v>-4.3801224489795898E-3</v>
       </c>
       <c r="G17">
-        <v>8.2662270531401003E-2</v>
+        <v>6.9841183673469406E-2</v>
       </c>
       <c r="H17">
-        <v>3.2897584541062802E-3</v>
+        <v>2.7795102040816299E-3</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2108,25 +2111,25 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>76.5</v>
+        <v>10.6163265306122</v>
       </c>
       <c r="C18">
-        <v>0.44361588235294103</v>
+        <v>6.1563020408163298E-2</v>
       </c>
       <c r="D18">
-        <v>-0.61764705882352899</v>
+        <v>-8.5714285714285701E-2</v>
       </c>
       <c r="E18">
-        <v>-6.2252941176470598E-3</v>
+        <v>-8.6391836734693898E-4</v>
       </c>
       <c r="F18">
-        <v>-5.9526470588235299E-2</v>
+        <v>-8.2608163265306105E-3</v>
       </c>
       <c r="G18">
-        <v>0.37798735294117602</v>
+        <v>5.2455387755102001E-2</v>
       </c>
       <c r="H18">
-        <v>1.9924999999999998E-2</v>
+        <v>2.7651020408163301E-3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2134,36 +2137,36 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>46.238738738738697</v>
+        <v>41.8979591836735</v>
       </c>
       <c r="C19">
-        <v>0.104333333333333</v>
+        <v>9.4538775510204107E-2</v>
       </c>
       <c r="D19">
-        <v>-8.1081081081081099E-2</v>
+        <v>-7.3469387755102006E-2</v>
       </c>
       <c r="E19">
-        <v>-1.8468468468468499E-4</v>
+        <v>-1.6734693877551001E-4</v>
       </c>
       <c r="F19">
-        <v>-6.6817567567567498E-3</v>
+        <v>-6.05448979591837E-3</v>
       </c>
       <c r="G19">
-        <v>9.7485135135135098E-2</v>
+        <v>8.8333469387755006E-2</v>
       </c>
       <c r="H19">
-        <v>5.34945945945946E-3</v>
+        <v>4.8472653061224502E-3</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B20">
-        <v>282.5</v>
+        <v>2.3061224489795902</v>
       </c>
       <c r="C20">
-        <v>2.909675</v>
+        <v>2.3752448979591799E-2</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2172,13 +2175,13 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>-0.39272499999999999</v>
+        <v>-3.2059183673469401E-3</v>
       </c>
       <c r="G20">
-        <v>2.51695</v>
+        <v>2.0546530612244901E-2</v>
       </c>
       <c r="H20">
-        <v>0.13824</v>
+        <v>1.1284897959183699E-3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2186,25 +2189,25 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>76.373626373626394</v>
+        <v>28.367346938775501</v>
       </c>
       <c r="C21">
-        <v>0.84476604395604404</v>
+        <v>0.31377024489795902</v>
       </c>
       <c r="D21">
-        <v>-1.0219780219780199</v>
+        <v>-0.37959183673469399</v>
       </c>
       <c r="E21">
-        <v>-4.5909230769230799E-2</v>
+        <v>-1.7052000000000001E-2</v>
       </c>
       <c r="F21">
-        <v>-6.6286483516483502E-2</v>
+        <v>-2.4620693877551E-2</v>
       </c>
       <c r="G21">
-        <v>0.73265307692307702</v>
+        <v>0.27212828571428599</v>
       </c>
       <c r="H21">
-        <v>3.6070879120879099E-2</v>
+        <v>1.33977551020408E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2212,10 +2215,10 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>4.8979591836734698E-2</v>
       </c>
       <c r="C22">
-        <v>2.9066666666666698E-3</v>
+        <v>1.4236734693877501E-4</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2227,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>2.9066666666666698E-3</v>
+        <v>1.4236734693877501E-4</v>
       </c>
       <c r="H22">
-        <v>1.5916666666666699E-4</v>
+        <v>7.7959183673469392E-6</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2238,25 +2241,25 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>10.7</v>
+        <v>0.43673469387755098</v>
       </c>
       <c r="C23">
-        <v>0.121907</v>
+        <v>4.9757959183673499E-3</v>
       </c>
       <c r="D23">
-        <v>-0.3</v>
+        <v>-1.2244897959183701E-2</v>
       </c>
       <c r="E23">
-        <v>-9.8829999999999994E-3</v>
+        <v>-4.0338775510204101E-4</v>
       </c>
       <c r="F23">
-        <v>-8.1200000000000005E-3</v>
+        <v>-3.31428571428571E-4</v>
       </c>
       <c r="G23">
-        <v>0.103904</v>
+        <v>4.24097959183674E-3</v>
       </c>
       <c r="H23">
-        <v>2.9369999999999999E-3</v>
+        <v>1.19877551020408E-4</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2264,10 +2267,10 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>1.6326530612244899E-2</v>
       </c>
       <c r="C24">
-        <v>2.0959999999999999E-2</v>
+        <v>3.4220408163265298E-4</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2276,13 +2279,13 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>-3.4975000000000002E-3</v>
+        <v>-5.7102040816326498E-5</v>
       </c>
       <c r="G24">
-        <v>1.7462499999999999E-2</v>
+        <v>2.8510204081632701E-4</v>
       </c>
       <c r="H24">
-        <v>9.6000000000000002E-4</v>
+        <v>1.5673469387755098E-5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2290,25 +2293,25 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>228.5</v>
+        <v>3.73061224489796</v>
       </c>
       <c r="C25">
-        <v>1.3322499999999999</v>
+        <v>2.1751020408163301E-2</v>
       </c>
       <c r="D25">
-        <v>-1.25</v>
+        <v>-2.04081632653061E-2</v>
       </c>
       <c r="E25">
-        <v>-5.4999999999999997E-3</v>
+        <v>-8.9795918367346894E-5</v>
       </c>
       <c r="F25">
-        <v>-1.0800000000000001E-2</v>
+        <v>-1.7632653061224501E-4</v>
       </c>
       <c r="G25">
-        <v>1.31595</v>
+        <v>2.1484897959183701E-2</v>
       </c>
       <c r="H25">
-        <v>7.2122500000000006E-2</v>
+        <v>1.17751020408163E-3</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2316,25 +2319,25 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>13.2443946188341</v>
+        <v>24.110204081632698</v>
       </c>
       <c r="C26">
-        <v>8.2733408071748699E-2</v>
+        <v>0.15060857142857101</v>
       </c>
       <c r="D26">
-        <v>-0.139013452914798</v>
+        <v>-0.25306122448979601</v>
       </c>
       <c r="E26">
-        <v>-3.8594170403587402E-3</v>
+        <v>-7.0257142857142896E-3</v>
       </c>
       <c r="F26">
-        <v>-1.26157847533632E-2</v>
+        <v>-2.2965877551020399E-2</v>
       </c>
       <c r="G26">
-        <v>6.6272466367713001E-2</v>
+        <v>0.12064293877550999</v>
       </c>
       <c r="H26">
-        <v>3.5254035874439501E-3</v>
+        <v>6.4176734693877696E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2342,25 +2345,25 @@
         <v>33</v>
       </c>
       <c r="B27">
-        <v>20.535714285714299</v>
+        <v>4.6938775510204103</v>
       </c>
       <c r="C27">
-        <v>0.15774589285714299</v>
+        <v>3.6056204081632598E-2</v>
       </c>
       <c r="D27">
-        <v>-0.19642857142857101</v>
+        <v>-4.4897959183673501E-2</v>
       </c>
       <c r="E27">
-        <v>-2.9221428571428601E-3</v>
+        <v>-6.6791836734693898E-4</v>
       </c>
       <c r="F27">
-        <v>-2.1614999999999999E-2</v>
+        <v>-4.9405714285714296E-3</v>
       </c>
       <c r="G27">
-        <v>0.13320874999999999</v>
+        <v>3.04477142857143E-2</v>
       </c>
       <c r="H27">
-        <v>6.60160714285714E-3</v>
+        <v>1.5089387755101999E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2368,19 +2371,19 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>1.3333333333333299</v>
+        <v>1.6326530612244899E-2</v>
       </c>
       <c r="C28">
-        <v>4.4999999999999998E-2</v>
+        <v>5.5102040816326495E-4</v>
       </c>
       <c r="D28">
-        <v>-0.33333333333333298</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E28">
-        <v>-3.3333333333333298E-2</v>
+        <v>-4.0816326530612198E-4</v>
       </c>
       <c r="F28">
-        <v>-1.16666666666667E-2</v>
+        <v>-1.42857142857143E-4</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -2394,10 +2397,10 @@
         <v>35</v>
       </c>
       <c r="B29">
-        <v>2.0555555555555598</v>
+        <v>0.30204081632653101</v>
       </c>
       <c r="C29">
-        <v>4.3922777777777797E-2</v>
+        <v>6.4539591836734701E-3</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -2406,13 +2409,13 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>-1.89194444444444E-3</v>
+        <v>-2.7799999999999998E-4</v>
       </c>
       <c r="G29">
-        <v>4.2030833333333302E-2</v>
+        <v>6.1759591836734696E-3</v>
       </c>
       <c r="H29">
-        <v>2.3122222222222199E-3</v>
+        <v>3.3975510204081603E-4</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2420,25 +2423,25 @@
         <v>36</v>
       </c>
       <c r="B30">
-        <v>13.8780487804878</v>
+        <v>4.6448979591836697</v>
       </c>
       <c r="C30">
-        <v>7.2489390243902399E-2</v>
+        <v>2.4261755102040799E-2</v>
       </c>
       <c r="D30">
-        <v>-0.219512195121951</v>
+        <v>-7.3469387755102006E-2</v>
       </c>
       <c r="E30">
-        <v>-2.43085365853659E-3</v>
+        <v>-8.1359183673469402E-4</v>
       </c>
       <c r="F30">
-        <v>-3.8576829268292699E-3</v>
+        <v>-1.2911428571428601E-3</v>
       </c>
       <c r="G30">
-        <v>6.6261829268292605E-2</v>
+        <v>2.2177428571428601E-2</v>
       </c>
       <c r="H30">
-        <v>2.2417073170731701E-3</v>
+        <v>7.5028571428571397E-4</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2446,10 +2449,10 @@
         <v>37</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>3.2653061224489799E-2</v>
       </c>
       <c r="C31">
-        <v>0.04</v>
+        <v>1.6326530612244901E-4</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -2461,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0.04</v>
+        <v>1.6326530612244901E-4</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2472,22 +2475,22 @@
         <v>38</v>
       </c>
       <c r="B32">
-        <v>95</v>
+        <v>0.77551020408163296</v>
       </c>
       <c r="C32">
-        <v>9.9500000000000005E-2</v>
+        <v>8.1224489795918395E-4</v>
       </c>
       <c r="D32">
-        <v>-1.5</v>
+        <v>-1.2244897959183701E-2</v>
       </c>
       <c r="E32">
-        <v>-1.5E-3</v>
+        <v>-1.22448979591837E-5</v>
       </c>
       <c r="F32">
-        <v>-5.2350000000000001E-3</v>
+        <v>-4.2734693877550999E-5</v>
       </c>
       <c r="G32">
-        <v>9.2765E-2</v>
+        <v>7.5726530612244903E-4</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2498,10 +2501,10 @@
         <v>39</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>8.1632653061224497E-3</v>
       </c>
       <c r="C33">
-        <v>9.9979999999999999E-2</v>
+        <v>4.0808163265306099E-4</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -2510,13 +2513,13 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>-3.6299999999999999E-2</v>
+        <v>-1.48163265306122E-4</v>
       </c>
       <c r="G33">
-        <v>6.368E-2</v>
+        <v>2.5991836734693899E-4</v>
       </c>
       <c r="H33">
-        <v>3.5000000000000001E-3</v>
+        <v>1.4285714285714301E-5</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2524,25 +2527,25 @@
         <v>40</v>
       </c>
       <c r="B34">
-        <v>1.62903225806452</v>
+        <v>0.41224489795918401</v>
       </c>
       <c r="C34">
-        <v>3.4011290322580698E-2</v>
+        <v>8.6069387755102096E-3</v>
       </c>
       <c r="D34">
-        <v>-3.2258064516128997E-2</v>
+        <v>-8.1632653061224497E-3</v>
       </c>
       <c r="E34">
-        <v>-1.1169354838709701E-3</v>
+        <v>-2.8265306122449E-4</v>
       </c>
       <c r="F34">
-        <v>-5.8199999999999997E-3</v>
+        <v>-1.4728163265306099E-3</v>
       </c>
       <c r="G34">
-        <v>2.7265967741935501E-2</v>
+        <v>6.8999591836734703E-3</v>
       </c>
       <c r="H34">
-        <v>1.2719354838709701E-3</v>
+        <v>3.2187755102040799E-4</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2550,25 +2553,25 @@
         <v>41</v>
       </c>
       <c r="B35">
-        <v>72.571428571428598</v>
+        <v>8.2938775510204099</v>
       </c>
       <c r="C35">
-        <v>0.31304357142857098</v>
+        <v>3.57764081632653E-2</v>
       </c>
       <c r="D35">
-        <v>-3.5714285714285698E-2</v>
+        <v>-4.0816326530612197E-3</v>
       </c>
       <c r="E35">
-        <v>-1.4249999999999999E-4</v>
+        <v>-1.62857142857143E-5</v>
       </c>
       <c r="F35">
-        <v>-2.2925714285714299E-2</v>
+        <v>-2.6200816326530599E-3</v>
       </c>
       <c r="G35">
-        <v>0.28997535714285699</v>
+        <v>3.3140040816326502E-2</v>
       </c>
       <c r="H35">
-        <v>1.46171428571429E-2</v>
+        <v>1.6705306122448999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>